<commit_message>
Organize ODR utils and create black body radiation analysis notebook
</commit_message>
<xml_diff>
--- a/data/black_body_radiation_spectrum.xlsx
+++ b/data/black_body_radiation_spectrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gadi.bessudo/Library/CloudStorage/GoogleDrive-gadibessudo@gmail.com/My Drive/Projects/University/Lab C/2025a/WaveParticleDuality/wave-particle-duality-experiment-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C491977B-5C5D-6E41-B0FC-1D9C044CD03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76013A9-7773-9741-87FA-3B54FA791A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{42811CE2-A1BB-A54D-9016-A5B1765426A4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="starting_angle" sheetId="3" r:id="rId2"/>
     <sheet name="lightbulb_four_wires" sheetId="4" r:id="rId3"/>
     <sheet name="lightbulb_resistance_low_temp" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
+    <sheet name="max_intensity_angle" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -730,7 +730,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>